<commit_message>
Periodo and User Controller finally api.php
</commit_message>
<xml_diff>
--- a/public/FIN13Final.xlsx
+++ b/public/FIN13Final.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>PLAN OPERATIVO DE GRUPOS Y SEMILLEROS DE INVESTIGACIÓN</t>
   </si>
@@ -84,7 +84,22 @@
     <t>alguno</t>
   </si>
   <si>
-    <t>se realizó</t>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>maicol es el mejor tipo que conozco</t>
+  </si>
+  <si>
+    <t>maicol</t>
+  </si>
+  <si>
+    <t>$$$</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>billetera</t>
   </si>
   <si>
     <t xml:space="preserve">HORARIO DE REUNIÓN: </t>
@@ -1090,16 +1105,30 @@
       <c r="CK10" s="5"/>
     </row>
     <row r="11" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="G11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1755,7 +1784,7 @@
     </row>
     <row r="21" spans="1:89" customHeight="1" ht="18.75">
       <c r="A21" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3189,7 +3218,7 @@
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -3322,7 +3351,7 @@
     </row>
     <row r="4" spans="1:45" customHeight="1" ht="15">
       <c r="A4" s="18" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -3331,53 +3360,53 @@
     </row>
     <row r="5" spans="1:45" customHeight="1" ht="38.25">
       <c r="A5" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:45" customHeight="1" ht="15">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:45" customHeight="1" ht="15">
       <c r="A7" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D7" s="7">
         <v>11235796</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:45" customHeight="1" ht="15">
@@ -3608,7 +3637,7 @@
     </row>
     <row r="18" spans="1:45" customHeight="1" ht="15">
       <c r="A18" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3"/>
     </row>

</xml_diff>

<commit_message>
Adding showPorPeriodoActividad to periodoController
</commit_message>
<xml_diff>
--- a/public/FIN13Final.xlsx
+++ b/public/FIN13Final.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>PLAN OPERATIVO DE GRUPOS Y SEMILLEROS DE INVESTIGACIÓN</t>
   </si>
@@ -30,16 +30,19 @@
     <t>NOMBRE DEL GRUPO Y/O SEMILLERO DE INVESTIGACIÓN</t>
   </si>
   <si>
+    <t>qqqqqqqqqq</t>
+  </si>
+  <si>
     <t>DIRECTOR DEL GRUPO Y/O SEMILLERO</t>
   </si>
   <si>
-    <t>José Alejandro Cortés Taborda</t>
+    <t>Prueba Coordinador</t>
   </si>
   <si>
     <t>SEMESTRE</t>
   </si>
   <si>
-    <t>2019-2</t>
+    <t>2020-1</t>
   </si>
   <si>
     <t>ACTIVIDAD</t>
@@ -60,46 +63,34 @@
     <t>PRODUCTO</t>
   </si>
   <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
-    <t>S</t>
+    <t>J</t>
   </si>
   <si>
-    <t>O</t>
+    <t>Actividad 1</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Brayan Legarda</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>yo</t>
-  </si>
-  <si>
-    <t>alguno</t>
-  </si>
-  <si>
-    <t>Activo</t>
-  </si>
-  <si>
-    <t>maicol es el mejor tipo que conozco</t>
-  </si>
-  <si>
-    <t>maicol</t>
-  </si>
-  <si>
-    <t>$$$</t>
+    <t>Aula</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>billetera</t>
+    <t>FH05</t>
+  </si>
+  <si>
+    <t>No se realizó</t>
   </si>
   <si>
     <t xml:space="preserve">HORARIO DE REUNIÓN: </t>
@@ -126,28 +117,13 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Prueba Estudiante@1 Prueba@1</t>
+    <t>David Vergara</t>
   </si>
   <si>
     <t>Estudiante</t>
   </si>
   <si>
-    <t>5412@1</t>
-  </si>
-  <si>
-    <t>2132@q</t>
-  </si>
-  <si>
-    <t>prueba@pruebita.com</t>
-  </si>
-  <si>
-    <t>Integrante F3¾123 Integrante F3¾12</t>
-  </si>
-  <si>
-    <t>12║▀─▀║ÖIBz3</t>
-  </si>
-  <si>
-    <t>Integrante@gmail.com</t>
+    <t>david_vergara82141@elpoli.edu.co</t>
   </si>
   <si>
     <r>
@@ -916,8 +892,8 @@
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
-      <c r="E4" s="12">
-        <v>1</v>
+      <c r="E4" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -927,13 +903,13 @@
     </row>
     <row r="5" spans="1:89" customHeight="1" ht="15">
       <c r="A5" s="16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -943,13 +919,13 @@
     </row>
     <row r="6" spans="1:89" customHeight="1" ht="15">
       <c r="A6" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -959,26 +935,26 @@
     </row>
     <row r="8" spans="1:89" customHeight="1" ht="14.25">
       <c r="A8" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:89" customHeight="1" ht="15">
@@ -986,16 +962,16 @@
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>18</v>
@@ -1014,15 +990,21 @@
         <v>21</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1105,30 +1087,16 @@
       <c r="CK10" s="5"/>
     </row>
     <row r="11" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1784,7 +1752,7 @@
     </row>
     <row r="21" spans="1:89" customHeight="1" ht="18.75">
       <c r="A21" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3218,7 +3186,7 @@
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -3351,7 +3319,7 @@
     </row>
     <row r="4" spans="1:45" customHeight="1" ht="15">
       <c r="A4" s="18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -3360,54 +3328,44 @@
     </row>
     <row r="5" spans="1:45" customHeight="1" ht="38.25">
       <c r="A5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:45" customHeight="1" ht="15">
       <c r="A6" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="C6" s="7">
+        <v>147</v>
+      </c>
+      <c r="D6" s="7">
+        <v>147</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:45" customHeight="1" ht="15">
-      <c r="A7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="7">
-        <v>11235796</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:45" customHeight="1" ht="15">
       <c r="A8" s="7"/>
@@ -3637,7 +3595,7 @@
     </row>
     <row r="18" spans="1:45" customHeight="1" ht="15">
       <c r="A18" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3"/>
     </row>

</xml_diff>

<commit_message>
adding more space in semillerostable
</commit_message>
<xml_diff>
--- a/public/FIN13Final.xlsx
+++ b/public/FIN13Final.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>PLAN OPERATIVO DE GRUPOS Y SEMILLEROS DE INVESTIGACIÓN</t>
   </si>
@@ -30,19 +30,19 @@
     <t>NOMBRE DEL GRUPO Y/O SEMILLERO DE INVESTIGACIÓN</t>
   </si>
   <si>
-    <t>SIIC (Semillero de Investigación en Inteligencia Computacional)</t>
+    <t>Semillero de Investigación en Inteligencia Computacional</t>
   </si>
   <si>
     <t>DIRECTOR DEL GRUPO Y/O SEMILLERO</t>
   </si>
   <si>
-    <t>Prueba Coordinador</t>
+    <t>José Alejandro Cortés Taborda</t>
   </si>
   <si>
     <t>SEMESTRE</t>
   </si>
   <si>
-    <t>2020-1</t>
+    <t>2019-2</t>
   </si>
   <si>
     <t>ACTIVIDAD</t>
@@ -63,16 +63,19 @@
     <t>PRODUCTO</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>J</t>
+    <t>S</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>Actividad 1</t>
@@ -90,7 +93,7 @@
     <t>FH05</t>
   </si>
   <si>
-    <t>No se realizó</t>
+    <t>Se realizó</t>
   </si>
   <si>
     <t xml:space="preserve">HORARIO DE REUNIÓN: </t>
@@ -117,13 +120,13 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>David Vergara</t>
+    <t>Usuario nuevo Prueba</t>
   </si>
   <si>
     <t>Estudiante</t>
   </si>
   <si>
-    <t>david_vergara82141@elpoli.edu.co</t>
+    <t>Usuario_prueba@elpoli.edu.co</t>
   </si>
   <si>
     <r>
@@ -971,40 +974,38 @@
         <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
       <c r="A10" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1752,7 +1753,7 @@
     </row>
     <row r="21" spans="1:89" customHeight="1" ht="18.75">
       <c r="A21" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3186,7 +3187,7 @@
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -3319,7 +3320,7 @@
     </row>
     <row r="4" spans="1:45" customHeight="1" ht="15">
       <c r="A4" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -3328,36 +3329,36 @@
     </row>
     <row r="5" spans="1:45" customHeight="1" ht="38.25">
       <c r="A5" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:45" customHeight="1" ht="15">
       <c r="A6" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="7">
-        <v>147</v>
+        <v>1002</v>
       </c>
       <c r="D6" s="7">
-        <v>147</v>
+        <v>1002</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:45" customHeight="1" ht="15">
@@ -3595,7 +3596,7 @@
     </row>
     <row r="18" spans="1:45" customHeight="1" ht="15">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3"/>
     </row>

</xml_diff>

<commit_message>
Final changes in pdf
</commit_message>
<xml_diff>
--- a/public/FIN13Final.xlsx
+++ b/public/FIN13Final.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>PLAN OPERATIVO DE GRUPOS Y SEMILLEROS DE INVESTIGACIÓN</t>
   </si>
@@ -36,7 +36,7 @@
     <t>DIRECTOR DEL GRUPO Y/O SEMILLERO</t>
   </si>
   <si>
-    <t>José Alejandro Cortés Taborda</t>
+    <t>Alejandro Cortés</t>
   </si>
   <si>
     <t>SEMESTRE</t>
@@ -78,10 +78,10 @@
     <t>D</t>
   </si>
   <si>
-    <t>Actividad 1</t>
+    <t>Sustentación</t>
   </si>
   <si>
-    <t>Brayan Legarda</t>
+    <t>Brayan Legarda y Alejandro Cortés</t>
   </si>
   <si>
     <t>Aula</t>
@@ -90,7 +90,7 @@
     <t>X</t>
   </si>
   <si>
-    <t>FH05</t>
+    <t>Jurados</t>
   </si>
   <si>
     <t>Se realizó</t>
@@ -120,13 +120,19 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Usuario nuevo Prueba</t>
+    <t>Camila Corrales</t>
   </si>
   <si>
     <t>Estudiante</t>
   </si>
   <si>
-    <t>Usuario_prueba@elpoli.edu.co</t>
+    <t>camila_corrales@elpoli.edu.co</t>
+  </si>
+  <si>
+    <t>Int Prueba</t>
+  </si>
+  <si>
+    <t>pruebai@elpoli.edu.co</t>
   </si>
   <si>
     <r>
@@ -283,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
@@ -326,6 +332,14 @@
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
@@ -405,7 +419,7 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>657634</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1428750" cy="685800"/>
@@ -759,10 +773,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:CK1101"/>
+  <dimension ref="A1:CK1110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="10" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -859,111 +873,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:89" customHeight="1" ht="15">
-      <c r="A1" s="12"/>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:89" customHeight="1" ht="17.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:89" customHeight="1" ht="15">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="12" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:89" customHeight="1" ht="15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="12" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:89" customHeight="1" ht="15">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="12" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="8" spans="1:89" customHeight="1" ht="14.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:89" customHeight="1" ht="15">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
@@ -979,32 +993,32 @@
       <c r="H9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="11" t="s">
         <v>25</v>
       </c>
       <c r="K10" s="5"/>
@@ -1088,16 +1102,16 @@
       <c r="CK10" s="5"/>
     </row>
     <row r="11" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -1179,16 +1193,16 @@
       <c r="CK11" s="5"/>
     </row>
     <row r="12" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1270,16 +1284,16 @@
       <c r="CK12" s="5"/>
     </row>
     <row r="13" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -1361,16 +1375,16 @@
       <c r="CK13" s="5"/>
     </row>
     <row r="14" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -1452,16 +1466,16 @@
       <c r="CK14" s="5"/>
     </row>
     <row r="15" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1724,130 +1738,839 @@
       <c r="CJ17" s="5"/>
       <c r="CK17" s="5"/>
     </row>
-    <row r="18" spans="1:89" customHeight="1" ht="15">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:89" customHeight="1" ht="15">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:89" customHeight="1" ht="15">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:89" customHeight="1" ht="18.75">
-      <c r="A21" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:89" customHeight="1" ht="15">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:89" customHeight="1" ht="15">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:89" customHeight="1" ht="15">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:89" customHeight="1" ht="15">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:89" customHeight="1" ht="15">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
+    <row r="18" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="5"/>
+      <c r="AQ18" s="5"/>
+      <c r="AR18" s="5"/>
+      <c r="AS18" s="5"/>
+      <c r="AT18" s="5"/>
+      <c r="AU18" s="5"/>
+      <c r="AV18" s="5"/>
+      <c r="AW18" s="5"/>
+      <c r="AX18" s="5"/>
+      <c r="AY18" s="5"/>
+      <c r="AZ18" s="5"/>
+      <c r="BA18" s="5"/>
+      <c r="BB18" s="5"/>
+      <c r="BC18" s="5"/>
+      <c r="BD18" s="5"/>
+      <c r="BE18" s="5"/>
+      <c r="BF18" s="5"/>
+      <c r="BG18" s="5"/>
+      <c r="BH18" s="5"/>
+      <c r="BI18" s="5"/>
+      <c r="BJ18" s="5"/>
+      <c r="BK18" s="5"/>
+      <c r="BL18" s="5"/>
+      <c r="BM18" s="5"/>
+      <c r="BN18" s="5"/>
+      <c r="BO18" s="5"/>
+      <c r="BP18" s="5"/>
+      <c r="BQ18" s="5"/>
+      <c r="BR18" s="5"/>
+      <c r="BS18" s="5"/>
+      <c r="BT18" s="5"/>
+      <c r="BU18" s="5"/>
+      <c r="BV18" s="5"/>
+      <c r="BW18" s="5"/>
+      <c r="BX18" s="5"/>
+      <c r="BY18" s="5"/>
+      <c r="BZ18" s="5"/>
+      <c r="CA18" s="5"/>
+      <c r="CB18" s="5"/>
+      <c r="CC18" s="5"/>
+      <c r="CD18" s="5"/>
+      <c r="CE18" s="5"/>
+      <c r="CF18" s="5"/>
+      <c r="CG18" s="5"/>
+      <c r="CH18" s="5"/>
+      <c r="CI18" s="5"/>
+      <c r="CJ18" s="5"/>
+      <c r="CK18" s="5"/>
+    </row>
+    <row r="19" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="5"/>
+      <c r="AQ19" s="5"/>
+      <c r="AR19" s="5"/>
+      <c r="AS19" s="5"/>
+      <c r="AT19" s="5"/>
+      <c r="AU19" s="5"/>
+      <c r="AV19" s="5"/>
+      <c r="AW19" s="5"/>
+      <c r="AX19" s="5"/>
+      <c r="AY19" s="5"/>
+      <c r="AZ19" s="5"/>
+      <c r="BA19" s="5"/>
+      <c r="BB19" s="5"/>
+      <c r="BC19" s="5"/>
+      <c r="BD19" s="5"/>
+      <c r="BE19" s="5"/>
+      <c r="BF19" s="5"/>
+      <c r="BG19" s="5"/>
+      <c r="BH19" s="5"/>
+      <c r="BI19" s="5"/>
+      <c r="BJ19" s="5"/>
+      <c r="BK19" s="5"/>
+      <c r="BL19" s="5"/>
+      <c r="BM19" s="5"/>
+      <c r="BN19" s="5"/>
+      <c r="BO19" s="5"/>
+      <c r="BP19" s="5"/>
+      <c r="BQ19" s="5"/>
+      <c r="BR19" s="5"/>
+      <c r="BS19" s="5"/>
+      <c r="BT19" s="5"/>
+      <c r="BU19" s="5"/>
+      <c r="BV19" s="5"/>
+      <c r="BW19" s="5"/>
+      <c r="BX19" s="5"/>
+      <c r="BY19" s="5"/>
+      <c r="BZ19" s="5"/>
+      <c r="CA19" s="5"/>
+      <c r="CB19" s="5"/>
+      <c r="CC19" s="5"/>
+      <c r="CD19" s="5"/>
+      <c r="CE19" s="5"/>
+      <c r="CF19" s="5"/>
+      <c r="CG19" s="5"/>
+      <c r="CH19" s="5"/>
+      <c r="CI19" s="5"/>
+      <c r="CJ19" s="5"/>
+      <c r="CK19" s="5"/>
+    </row>
+    <row r="20" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+      <c r="AG20" s="5"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="5"/>
+      <c r="AJ20" s="5"/>
+      <c r="AK20" s="5"/>
+      <c r="AL20" s="5"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="5"/>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="5"/>
+      <c r="AQ20" s="5"/>
+      <c r="AR20" s="5"/>
+      <c r="AS20" s="5"/>
+      <c r="AT20" s="5"/>
+      <c r="AU20" s="5"/>
+      <c r="AV20" s="5"/>
+      <c r="AW20" s="5"/>
+      <c r="AX20" s="5"/>
+      <c r="AY20" s="5"/>
+      <c r="AZ20" s="5"/>
+      <c r="BA20" s="5"/>
+      <c r="BB20" s="5"/>
+      <c r="BC20" s="5"/>
+      <c r="BD20" s="5"/>
+      <c r="BE20" s="5"/>
+      <c r="BF20" s="5"/>
+      <c r="BG20" s="5"/>
+      <c r="BH20" s="5"/>
+      <c r="BI20" s="5"/>
+      <c r="BJ20" s="5"/>
+      <c r="BK20" s="5"/>
+      <c r="BL20" s="5"/>
+      <c r="BM20" s="5"/>
+      <c r="BN20" s="5"/>
+      <c r="BO20" s="5"/>
+      <c r="BP20" s="5"/>
+      <c r="BQ20" s="5"/>
+      <c r="BR20" s="5"/>
+      <c r="BS20" s="5"/>
+      <c r="BT20" s="5"/>
+      <c r="BU20" s="5"/>
+      <c r="BV20" s="5"/>
+      <c r="BW20" s="5"/>
+      <c r="BX20" s="5"/>
+      <c r="BY20" s="5"/>
+      <c r="BZ20" s="5"/>
+      <c r="CA20" s="5"/>
+      <c r="CB20" s="5"/>
+      <c r="CC20" s="5"/>
+      <c r="CD20" s="5"/>
+      <c r="CE20" s="5"/>
+      <c r="CF20" s="5"/>
+      <c r="CG20" s="5"/>
+      <c r="CH20" s="5"/>
+      <c r="CI20" s="5"/>
+      <c r="CJ20" s="5"/>
+      <c r="CK20" s="5"/>
+    </row>
+    <row r="21" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
+      <c r="AH21" s="5"/>
+      <c r="AI21" s="5"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="5"/>
+      <c r="AO21" s="5"/>
+      <c r="AP21" s="5"/>
+      <c r="AQ21" s="5"/>
+      <c r="AR21" s="5"/>
+      <c r="AS21" s="5"/>
+      <c r="AT21" s="5"/>
+      <c r="AU21" s="5"/>
+      <c r="AV21" s="5"/>
+      <c r="AW21" s="5"/>
+      <c r="AX21" s="5"/>
+      <c r="AY21" s="5"/>
+      <c r="AZ21" s="5"/>
+      <c r="BA21" s="5"/>
+      <c r="BB21" s="5"/>
+      <c r="BC21" s="5"/>
+      <c r="BD21" s="5"/>
+      <c r="BE21" s="5"/>
+      <c r="BF21" s="5"/>
+      <c r="BG21" s="5"/>
+      <c r="BH21" s="5"/>
+      <c r="BI21" s="5"/>
+      <c r="BJ21" s="5"/>
+      <c r="BK21" s="5"/>
+      <c r="BL21" s="5"/>
+      <c r="BM21" s="5"/>
+      <c r="BN21" s="5"/>
+      <c r="BO21" s="5"/>
+      <c r="BP21" s="5"/>
+      <c r="BQ21" s="5"/>
+      <c r="BR21" s="5"/>
+      <c r="BS21" s="5"/>
+      <c r="BT21" s="5"/>
+      <c r="BU21" s="5"/>
+      <c r="BV21" s="5"/>
+      <c r="BW21" s="5"/>
+      <c r="BX21" s="5"/>
+      <c r="BY21" s="5"/>
+      <c r="BZ21" s="5"/>
+      <c r="CA21" s="5"/>
+      <c r="CB21" s="5"/>
+      <c r="CC21" s="5"/>
+      <c r="CD21" s="5"/>
+      <c r="CE21" s="5"/>
+      <c r="CF21" s="5"/>
+      <c r="CG21" s="5"/>
+      <c r="CH21" s="5"/>
+      <c r="CI21" s="5"/>
+      <c r="CJ21" s="5"/>
+      <c r="CK21" s="5"/>
+    </row>
+    <row r="22" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="5"/>
+      <c r="AJ22" s="5"/>
+      <c r="AK22" s="5"/>
+      <c r="AL22" s="5"/>
+      <c r="AM22" s="5"/>
+      <c r="AN22" s="5"/>
+      <c r="AO22" s="5"/>
+      <c r="AP22" s="5"/>
+      <c r="AQ22" s="5"/>
+      <c r="AR22" s="5"/>
+      <c r="AS22" s="5"/>
+      <c r="AT22" s="5"/>
+      <c r="AU22" s="5"/>
+      <c r="AV22" s="5"/>
+      <c r="AW22" s="5"/>
+      <c r="AX22" s="5"/>
+      <c r="AY22" s="5"/>
+      <c r="AZ22" s="5"/>
+      <c r="BA22" s="5"/>
+      <c r="BB22" s="5"/>
+      <c r="BC22" s="5"/>
+      <c r="BD22" s="5"/>
+      <c r="BE22" s="5"/>
+      <c r="BF22" s="5"/>
+      <c r="BG22" s="5"/>
+      <c r="BH22" s="5"/>
+      <c r="BI22" s="5"/>
+      <c r="BJ22" s="5"/>
+      <c r="BK22" s="5"/>
+      <c r="BL22" s="5"/>
+      <c r="BM22" s="5"/>
+      <c r="BN22" s="5"/>
+      <c r="BO22" s="5"/>
+      <c r="BP22" s="5"/>
+      <c r="BQ22" s="5"/>
+      <c r="BR22" s="5"/>
+      <c r="BS22" s="5"/>
+      <c r="BT22" s="5"/>
+      <c r="BU22" s="5"/>
+      <c r="BV22" s="5"/>
+      <c r="BW22" s="5"/>
+      <c r="BX22" s="5"/>
+      <c r="BY22" s="5"/>
+      <c r="BZ22" s="5"/>
+      <c r="CA22" s="5"/>
+      <c r="CB22" s="5"/>
+      <c r="CC22" s="5"/>
+      <c r="CD22" s="5"/>
+      <c r="CE22" s="5"/>
+      <c r="CF22" s="5"/>
+      <c r="CG22" s="5"/>
+      <c r="CH22" s="5"/>
+      <c r="CI22" s="5"/>
+      <c r="CJ22" s="5"/>
+      <c r="CK22" s="5"/>
+    </row>
+    <row r="23" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="5"/>
+      <c r="AH23" s="5"/>
+      <c r="AI23" s="5"/>
+      <c r="AJ23" s="5"/>
+      <c r="AK23" s="5"/>
+      <c r="AL23" s="5"/>
+      <c r="AM23" s="5"/>
+      <c r="AN23" s="5"/>
+      <c r="AO23" s="5"/>
+      <c r="AP23" s="5"/>
+      <c r="AQ23" s="5"/>
+      <c r="AR23" s="5"/>
+      <c r="AS23" s="5"/>
+      <c r="AT23" s="5"/>
+      <c r="AU23" s="5"/>
+      <c r="AV23" s="5"/>
+      <c r="AW23" s="5"/>
+      <c r="AX23" s="5"/>
+      <c r="AY23" s="5"/>
+      <c r="AZ23" s="5"/>
+      <c r="BA23" s="5"/>
+      <c r="BB23" s="5"/>
+      <c r="BC23" s="5"/>
+      <c r="BD23" s="5"/>
+      <c r="BE23" s="5"/>
+      <c r="BF23" s="5"/>
+      <c r="BG23" s="5"/>
+      <c r="BH23" s="5"/>
+      <c r="BI23" s="5"/>
+      <c r="BJ23" s="5"/>
+      <c r="BK23" s="5"/>
+      <c r="BL23" s="5"/>
+      <c r="BM23" s="5"/>
+      <c r="BN23" s="5"/>
+      <c r="BO23" s="5"/>
+      <c r="BP23" s="5"/>
+      <c r="BQ23" s="5"/>
+      <c r="BR23" s="5"/>
+      <c r="BS23" s="5"/>
+      <c r="BT23" s="5"/>
+      <c r="BU23" s="5"/>
+      <c r="BV23" s="5"/>
+      <c r="BW23" s="5"/>
+      <c r="BX23" s="5"/>
+      <c r="BY23" s="5"/>
+      <c r="BZ23" s="5"/>
+      <c r="CA23" s="5"/>
+      <c r="CB23" s="5"/>
+      <c r="CC23" s="5"/>
+      <c r="CD23" s="5"/>
+      <c r="CE23" s="5"/>
+      <c r="CF23" s="5"/>
+      <c r="CG23" s="5"/>
+      <c r="CH23" s="5"/>
+      <c r="CI23" s="5"/>
+      <c r="CJ23" s="5"/>
+      <c r="CK23" s="5"/>
+    </row>
+    <row r="24" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
+      <c r="AG24" s="5"/>
+      <c r="AH24" s="5"/>
+      <c r="AI24" s="5"/>
+      <c r="AJ24" s="5"/>
+      <c r="AK24" s="5"/>
+      <c r="AL24" s="5"/>
+      <c r="AM24" s="5"/>
+      <c r="AN24" s="5"/>
+      <c r="AO24" s="5"/>
+      <c r="AP24" s="5"/>
+      <c r="AQ24" s="5"/>
+      <c r="AR24" s="5"/>
+      <c r="AS24" s="5"/>
+      <c r="AT24" s="5"/>
+      <c r="AU24" s="5"/>
+      <c r="AV24" s="5"/>
+      <c r="AW24" s="5"/>
+      <c r="AX24" s="5"/>
+      <c r="AY24" s="5"/>
+      <c r="AZ24" s="5"/>
+      <c r="BA24" s="5"/>
+      <c r="BB24" s="5"/>
+      <c r="BC24" s="5"/>
+      <c r="BD24" s="5"/>
+      <c r="BE24" s="5"/>
+      <c r="BF24" s="5"/>
+      <c r="BG24" s="5"/>
+      <c r="BH24" s="5"/>
+      <c r="BI24" s="5"/>
+      <c r="BJ24" s="5"/>
+      <c r="BK24" s="5"/>
+      <c r="BL24" s="5"/>
+      <c r="BM24" s="5"/>
+      <c r="BN24" s="5"/>
+      <c r="BO24" s="5"/>
+      <c r="BP24" s="5"/>
+      <c r="BQ24" s="5"/>
+      <c r="BR24" s="5"/>
+      <c r="BS24" s="5"/>
+      <c r="BT24" s="5"/>
+      <c r="BU24" s="5"/>
+      <c r="BV24" s="5"/>
+      <c r="BW24" s="5"/>
+      <c r="BX24" s="5"/>
+      <c r="BY24" s="5"/>
+      <c r="BZ24" s="5"/>
+      <c r="CA24" s="5"/>
+      <c r="CB24" s="5"/>
+      <c r="CC24" s="5"/>
+      <c r="CD24" s="5"/>
+      <c r="CE24" s="5"/>
+      <c r="CF24" s="5"/>
+      <c r="CG24" s="5"/>
+      <c r="CH24" s="5"/>
+      <c r="CI24" s="5"/>
+      <c r="CJ24" s="5"/>
+      <c r="CK24" s="5"/>
+    </row>
+    <row r="25" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="5"/>
+      <c r="AJ25" s="5"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="5"/>
+      <c r="AM25" s="5"/>
+      <c r="AN25" s="5"/>
+      <c r="AO25" s="5"/>
+      <c r="AP25" s="5"/>
+      <c r="AQ25" s="5"/>
+      <c r="AR25" s="5"/>
+      <c r="AS25" s="5"/>
+      <c r="AT25" s="5"/>
+      <c r="AU25" s="5"/>
+      <c r="AV25" s="5"/>
+      <c r="AW25" s="5"/>
+      <c r="AX25" s="5"/>
+      <c r="AY25" s="5"/>
+      <c r="AZ25" s="5"/>
+      <c r="BA25" s="5"/>
+      <c r="BB25" s="5"/>
+      <c r="BC25" s="5"/>
+      <c r="BD25" s="5"/>
+      <c r="BE25" s="5"/>
+      <c r="BF25" s="5"/>
+      <c r="BG25" s="5"/>
+      <c r="BH25" s="5"/>
+      <c r="BI25" s="5"/>
+      <c r="BJ25" s="5"/>
+      <c r="BK25" s="5"/>
+      <c r="BL25" s="5"/>
+      <c r="BM25" s="5"/>
+      <c r="BN25" s="5"/>
+      <c r="BO25" s="5"/>
+      <c r="BP25" s="5"/>
+      <c r="BQ25" s="5"/>
+      <c r="BR25" s="5"/>
+      <c r="BS25" s="5"/>
+      <c r="BT25" s="5"/>
+      <c r="BU25" s="5"/>
+      <c r="BV25" s="5"/>
+      <c r="BW25" s="5"/>
+      <c r="BX25" s="5"/>
+      <c r="BY25" s="5"/>
+      <c r="BZ25" s="5"/>
+      <c r="CA25" s="5"/>
+      <c r="CB25" s="5"/>
+      <c r="CC25" s="5"/>
+      <c r="CD25" s="5"/>
+      <c r="CE25" s="5"/>
+      <c r="CF25" s="5"/>
+      <c r="CG25" s="5"/>
+      <c r="CH25" s="5"/>
+      <c r="CI25" s="5"/>
+      <c r="CJ25" s="5"/>
+      <c r="CK25" s="5"/>
+    </row>
+    <row r="26" spans="1:89" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="5"/>
+      <c r="AO26" s="5"/>
+      <c r="AP26" s="5"/>
+      <c r="AQ26" s="5"/>
+      <c r="AR26" s="5"/>
+      <c r="AS26" s="5"/>
+      <c r="AT26" s="5"/>
+      <c r="AU26" s="5"/>
+      <c r="AV26" s="5"/>
+      <c r="AW26" s="5"/>
+      <c r="AX26" s="5"/>
+      <c r="AY26" s="5"/>
+      <c r="AZ26" s="5"/>
+      <c r="BA26" s="5"/>
+      <c r="BB26" s="5"/>
+      <c r="BC26" s="5"/>
+      <c r="BD26" s="5"/>
+      <c r="BE26" s="5"/>
+      <c r="BF26" s="5"/>
+      <c r="BG26" s="5"/>
+      <c r="BH26" s="5"/>
+      <c r="BI26" s="5"/>
+      <c r="BJ26" s="5"/>
+      <c r="BK26" s="5"/>
+      <c r="BL26" s="5"/>
+      <c r="BM26" s="5"/>
+      <c r="BN26" s="5"/>
+      <c r="BO26" s="5"/>
+      <c r="BP26" s="5"/>
+      <c r="BQ26" s="5"/>
+      <c r="BR26" s="5"/>
+      <c r="BS26" s="5"/>
+      <c r="BT26" s="5"/>
+      <c r="BU26" s="5"/>
+      <c r="BV26" s="5"/>
+      <c r="BW26" s="5"/>
+      <c r="BX26" s="5"/>
+      <c r="BY26" s="5"/>
+      <c r="BZ26" s="5"/>
+      <c r="CA26" s="5"/>
+      <c r="CB26" s="5"/>
+      <c r="CC26" s="5"/>
+      <c r="CD26" s="5"/>
+      <c r="CE26" s="5"/>
+      <c r="CF26" s="5"/>
+      <c r="CG26" s="5"/>
+      <c r="CH26" s="5"/>
+      <c r="CI26" s="5"/>
+      <c r="CJ26" s="5"/>
+      <c r="CK26" s="5"/>
     </row>
     <row r="27" spans="1:89" customHeight="1" ht="15">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:89" customHeight="1" ht="15">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
+      <c r="A28" s="1"/>
     </row>
     <row r="29" spans="1:89" customHeight="1" ht="15">
       <c r="A29" s="5"/>
@@ -1861,8 +2584,10 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:89" customHeight="1" ht="15">
-      <c r="A30" s="5"/>
+    <row r="30" spans="1:89" customHeight="1" ht="18.75">
+      <c r="A30" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1885,15 +2610,114 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="33" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="34" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="35" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="36" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="37" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="38" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="39" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="40" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="32" spans="1:89" customHeight="1" ht="15">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:89" customHeight="1" ht="15">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:89" customHeight="1" ht="15">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:89" customHeight="1" ht="15">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:89" customHeight="1" ht="15">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:89" customHeight="1" ht="15">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:89" customHeight="1" ht="15">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:89" customHeight="1" ht="15">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:89" customHeight="1" ht="15">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+    </row>
     <row r="41" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="42" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="43" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
@@ -2943,114 +3767,15 @@
     <row r="1087" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="1088" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="1089" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1090" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1090"/>
-      <c r="B1090"/>
-      <c r="C1090"/>
-      <c r="D1090"/>
-      <c r="E1090"/>
-      <c r="F1090"/>
-      <c r="G1090"/>
-      <c r="H1090"/>
-      <c r="I1090"/>
-      <c r="J1090"/>
-    </row>
-    <row r="1091" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1091"/>
-      <c r="B1091"/>
-      <c r="C1091"/>
-      <c r="D1091"/>
-      <c r="E1091"/>
-      <c r="F1091"/>
-      <c r="G1091"/>
-      <c r="H1091"/>
-      <c r="I1091"/>
-      <c r="J1091"/>
-    </row>
-    <row r="1092" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1092"/>
-      <c r="B1092"/>
-      <c r="C1092"/>
-      <c r="D1092"/>
-      <c r="E1092"/>
-      <c r="F1092"/>
-      <c r="G1092"/>
-      <c r="H1092"/>
-      <c r="I1092"/>
-      <c r="J1092"/>
-    </row>
-    <row r="1093" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1093"/>
-      <c r="B1093"/>
-      <c r="C1093"/>
-      <c r="D1093"/>
-      <c r="E1093"/>
-      <c r="F1093"/>
-      <c r="G1093"/>
-      <c r="H1093"/>
-      <c r="I1093"/>
-      <c r="J1093"/>
-    </row>
-    <row r="1094" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1094"/>
-      <c r="B1094"/>
-      <c r="C1094"/>
-      <c r="D1094"/>
-      <c r="E1094"/>
-      <c r="F1094"/>
-      <c r="G1094"/>
-      <c r="H1094"/>
-      <c r="I1094"/>
-      <c r="J1094"/>
-    </row>
-    <row r="1095" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1095"/>
-      <c r="B1095"/>
-      <c r="C1095"/>
-      <c r="D1095"/>
-      <c r="E1095"/>
-      <c r="F1095"/>
-      <c r="G1095"/>
-      <c r="H1095"/>
-      <c r="I1095"/>
-      <c r="J1095"/>
-    </row>
-    <row r="1096" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1096"/>
-      <c r="B1096"/>
-      <c r="C1096"/>
-      <c r="D1096"/>
-      <c r="E1096"/>
-      <c r="F1096"/>
-      <c r="G1096"/>
-      <c r="H1096"/>
-      <c r="I1096"/>
-      <c r="J1096"/>
-    </row>
-    <row r="1097" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1097"/>
-      <c r="B1097"/>
-      <c r="C1097"/>
-      <c r="D1097"/>
-      <c r="E1097"/>
-      <c r="F1097"/>
-      <c r="G1097"/>
-      <c r="H1097"/>
-      <c r="I1097"/>
-      <c r="J1097"/>
-    </row>
-    <row r="1098" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A1098"/>
-      <c r="B1098"/>
-      <c r="C1098"/>
-      <c r="D1098"/>
-      <c r="E1098"/>
-      <c r="F1098"/>
-      <c r="G1098"/>
-      <c r="H1098"/>
-      <c r="I1098"/>
-      <c r="J1098"/>
-    </row>
+    <row r="1090" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="1091" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="1092" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="1093" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="1094" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="1095" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="1096" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="1097" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="1098" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="1099" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
       <c r="A1099"/>
       <c r="B1099"/>
@@ -3086,6 +3811,114 @@
       <c r="H1101"/>
       <c r="I1101"/>
       <c r="J1101"/>
+    </row>
+    <row r="1102" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1102"/>
+      <c r="B1102"/>
+      <c r="C1102"/>
+      <c r="D1102"/>
+      <c r="E1102"/>
+      <c r="F1102"/>
+      <c r="G1102"/>
+      <c r="H1102"/>
+      <c r="I1102"/>
+      <c r="J1102"/>
+    </row>
+    <row r="1103" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1103"/>
+      <c r="B1103"/>
+      <c r="C1103"/>
+      <c r="D1103"/>
+      <c r="E1103"/>
+      <c r="F1103"/>
+      <c r="G1103"/>
+      <c r="H1103"/>
+      <c r="I1103"/>
+      <c r="J1103"/>
+    </row>
+    <row r="1104" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1104"/>
+      <c r="B1104"/>
+      <c r="C1104"/>
+      <c r="D1104"/>
+      <c r="E1104"/>
+      <c r="F1104"/>
+      <c r="G1104"/>
+      <c r="H1104"/>
+      <c r="I1104"/>
+      <c r="J1104"/>
+    </row>
+    <row r="1105" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1105"/>
+      <c r="B1105"/>
+      <c r="C1105"/>
+      <c r="D1105"/>
+      <c r="E1105"/>
+      <c r="F1105"/>
+      <c r="G1105"/>
+      <c r="H1105"/>
+      <c r="I1105"/>
+      <c r="J1105"/>
+    </row>
+    <row r="1106" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1106"/>
+      <c r="B1106"/>
+      <c r="C1106"/>
+      <c r="D1106"/>
+      <c r="E1106"/>
+      <c r="F1106"/>
+      <c r="G1106"/>
+      <c r="H1106"/>
+      <c r="I1106"/>
+      <c r="J1106"/>
+    </row>
+    <row r="1107" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1107"/>
+      <c r="B1107"/>
+      <c r="C1107"/>
+      <c r="D1107"/>
+      <c r="E1107"/>
+      <c r="F1107"/>
+      <c r="G1107"/>
+      <c r="H1107"/>
+      <c r="I1107"/>
+      <c r="J1107"/>
+    </row>
+    <row r="1108" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1108"/>
+      <c r="B1108"/>
+      <c r="C1108"/>
+      <c r="D1108"/>
+      <c r="E1108"/>
+      <c r="F1108"/>
+      <c r="G1108"/>
+      <c r="H1108"/>
+      <c r="I1108"/>
+      <c r="J1108"/>
+    </row>
+    <row r="1109" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1109"/>
+      <c r="B1109"/>
+      <c r="C1109"/>
+      <c r="D1109"/>
+      <c r="E1109"/>
+      <c r="F1109"/>
+      <c r="G1109"/>
+      <c r="H1109"/>
+      <c r="I1109"/>
+      <c r="J1109"/>
+    </row>
+    <row r="1110" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1">
+      <c r="A1110"/>
+      <c r="B1110"/>
+      <c r="C1110"/>
+      <c r="D1110"/>
+      <c r="E1110"/>
+      <c r="F1110"/>
+      <c r="G1110"/>
+      <c r="H1110"/>
+      <c r="I1110"/>
+      <c r="J1110"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="true" formatColumns="true" formatRows="true" insertColumns="true" insertRows="true" insertHyperlinks="true" deleteColumns="true" deleteRows="true" selectLockedCells="false" sort="true" autoFilter="true" pivotTables="true" selectUnlockedCells="false"/>
@@ -3125,10 +3958,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AS384"/>
+  <dimension ref="A1:AS390"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="10" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3180,12 +4013,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A1" s="12"/>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
@@ -3230,10 +4063,10 @@
       <c r="AS1" s="5"/>
     </row>
     <row r="2" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3319,13 +4152,13 @@
       <c r="AS3" s="5"/>
     </row>
     <row r="4" spans="1:45" customHeight="1" ht="15">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:45" customHeight="1" ht="38.25">
       <c r="A5" s="6" t="s">
@@ -3344,57 +4177,262 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:45" customHeight="1" ht="15">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="7">
-        <v>1002</v>
+      <c r="C6" s="12">
+        <v>11526</v>
       </c>
-      <c r="D6" s="7">
-        <v>1002</v>
+      <c r="D6" s="12">
+        <v>11526569</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" customHeight="1" ht="15">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:45" customHeight="1" ht="15">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:45" customHeight="1" ht="15">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:45" customHeight="1" ht="15">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+    </row>
+    <row r="7" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="12">
+        <v>45</v>
+      </c>
+      <c r="D7" s="12">
+        <v>4545</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+    </row>
+    <row r="8" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="5"/>
+      <c r="AP8" s="5"/>
+      <c r="AQ8" s="5"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="5"/>
+    </row>
+    <row r="9" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="5"/>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="5"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="5"/>
+      <c r="AQ9" s="5"/>
+      <c r="AR9" s="5"/>
+      <c r="AS9" s="5"/>
+    </row>
+    <row r="10" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="5"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="5"/>
     </row>
     <row r="11" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -3435,143 +4473,26 @@
       <c r="AR11" s="5"/>
       <c r="AS11" s="5"/>
     </row>
-    <row r="12" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+    <row r="12" spans="1:45" customHeight="1" ht="15">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
-      <c r="AG12" s="5"/>
-      <c r="AH12" s="5"/>
-      <c r="AI12" s="5"/>
-      <c r="AJ12" s="5"/>
-      <c r="AK12" s="5"/>
-      <c r="AL12" s="5"/>
-      <c r="AM12" s="5"/>
-      <c r="AN12" s="5"/>
-      <c r="AO12" s="5"/>
-      <c r="AP12" s="5"/>
-      <c r="AQ12" s="5"/>
-      <c r="AR12" s="5"/>
-      <c r="AS12" s="5"/>
-    </row>
-    <row r="13" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+    </row>
+    <row r="13" spans="1:45" customHeight="1" ht="15">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
-      <c r="W13" s="5"/>
-      <c r="X13" s="5"/>
-      <c r="Y13" s="5"/>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
-      <c r="AB13" s="5"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="5"/>
-      <c r="AE13" s="5"/>
-      <c r="AF13" s="5"/>
-      <c r="AG13" s="5"/>
-      <c r="AH13" s="5"/>
-      <c r="AI13" s="5"/>
-      <c r="AJ13" s="5"/>
-      <c r="AK13" s="5"/>
-      <c r="AL13" s="5"/>
-      <c r="AM13" s="5"/>
-      <c r="AN13" s="5"/>
-      <c r="AO13" s="5"/>
-      <c r="AP13" s="5"/>
-      <c r="AQ13" s="5"/>
-      <c r="AR13" s="5"/>
-      <c r="AS13" s="5"/>
-    </row>
-    <row r="14" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+    </row>
+    <row r="14" spans="1:45" customHeight="1" ht="15">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="5"/>
-      <c r="AH14" s="5"/>
-      <c r="AI14" s="5"/>
-      <c r="AJ14" s="5"/>
-      <c r="AK14" s="5"/>
-      <c r="AL14" s="5"/>
-      <c r="AM14" s="5"/>
-      <c r="AN14" s="5"/>
-      <c r="AO14" s="5"/>
-      <c r="AP14" s="5"/>
-      <c r="AQ14" s="5"/>
-      <c r="AR14" s="5"/>
-      <c r="AS14" s="5"/>
     </row>
     <row r="15" spans="1:45" customHeight="1" ht="15">
       <c r="A15" s="7"/>
@@ -3587,28 +4508,220 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:45" customHeight="1" ht="15">
+    <row r="17" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:45" customHeight="1" ht="15">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="5"/>
+      <c r="AO17" s="5"/>
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="5"/>
+      <c r="AR17" s="5"/>
+      <c r="AS17" s="5"/>
+    </row>
+    <row r="18" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="5"/>
+      <c r="AQ18" s="5"/>
+      <c r="AR18" s="5"/>
+      <c r="AS18" s="5"/>
+    </row>
+    <row r="19" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5"/>
+      <c r="AC19" s="5"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="5"/>
+      <c r="AI19" s="5"/>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
+      <c r="AP19" s="5"/>
+      <c r="AQ19" s="5"/>
+      <c r="AR19" s="5"/>
+      <c r="AS19" s="5"/>
+    </row>
+    <row r="20" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+      <c r="AG20" s="5"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="5"/>
+      <c r="AJ20" s="5"/>
+      <c r="AK20" s="5"/>
+      <c r="AL20" s="5"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="5"/>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="5"/>
+      <c r="AQ20" s="5"/>
+      <c r="AR20" s="5"/>
+      <c r="AS20" s="5"/>
+    </row>
+    <row r="21" spans="1:45" customHeight="1" ht="15">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:45" customHeight="1" ht="15">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:45" customHeight="1" ht="15">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:45" customHeight="1" ht="15">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
       </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="20" spans="1:45" customHeight="1" ht="14.25" s="5" customFormat="1"/>
-    <row r="21" spans="1:45" customHeight="1" ht="15" hidden="true" s="5" customFormat="1"/>
-    <row r="22" spans="1:45" customHeight="1" ht="15" hidden="true" s="5" customFormat="1"/>
-    <row r="23" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="24" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="25" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="26" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="27" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="28" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="26" spans="1:45" customHeight="1" ht="14.25" s="5" customFormat="1"/>
+    <row r="27" spans="1:45" customHeight="1" ht="15" hidden="true" s="5" customFormat="1"/>
+    <row r="28" spans="1:45" customHeight="1" ht="15" hidden="true" s="5" customFormat="1"/>
     <row r="29" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="30" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="31" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
@@ -3965,6 +5078,12 @@
     <row r="382" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="383" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="384" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="385" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="386" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="387" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="388" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="389" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
+    <row r="390" spans="1:45" customHeight="1" ht="15" s="5" customFormat="1"/>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="true" formatColumns="true" formatRows="true" insertColumns="true" insertRows="true" insertHyperlinks="true" deleteColumns="true" deleteRows="true" selectLockedCells="false" sort="true" autoFilter="true" pivotTables="true" selectUnlockedCells="false"/>
   <mergeCells>

</xml_diff>